<commit_message>
Signin and Signup done
</commit_message>
<xml_diff>
--- a/docs/网站页面流程.xlsx
+++ b/docs/网站页面流程.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B89DA7-29D9-403B-BA56-8B4D8F07B38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C086CCD-780B-41A8-9852-744505867F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,19 +26,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Main state(Loginstate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sub state</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -51,6 +43,14 @@
   </si>
   <si>
     <t>ImagePage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sign in state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unsign in state</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -124,25 +124,249 @@
 </file>
 
 <file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_1">
   <dgm:title val=""/>
   <dgm:desc val=""/>
   <dgm:catLst>
-    <dgm:cat type="accent1" pri="11200"/>
+    <dgm:cat type="accent1" pri="11100"/>
   </dgm:catLst>
   <dgm:styleLbl name="node0">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
+      <a:schemeClr val="lt1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
     <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="alignNode1">
+  <dgm:styleLbl name="node2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
@@ -151,132 +375,106 @@
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="node1">
+  <dgm:styleLbl name="callout">
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="accent1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="lnNode1">
-    <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="vennNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgImgPlace1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
     <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="alignImgPlace1">
+  <dgm:styleLbl name="asst0">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
     <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="bgImgPlace1">
+  <dgm:styleLbl name="asst1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
     <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </dgm:txFillClrLst>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans2D1">
+  <dgm:styleLbl name="asst2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="accent1">
         <a:tint val="60000"/>
@@ -292,146 +490,6 @@
     <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
-  <dgm:styleLbl name="fgSibTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgSibTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans1D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="callout">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst0">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
   <dgm:styleLbl name="parChTrans2D2">
     <dgm:fillClrLst meth="repeat">
       <a:schemeClr val="accent1"/>
@@ -441,9 +499,7 @@
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
+    <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="parChTrans2D3">
@@ -455,9 +511,7 @@
     </dgm:linClrLst>
     <dgm:effectClrLst/>
     <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
+    <dgm:txFillClrLst/>
     <dgm:txEffectClrLst/>
   </dgm:styleLbl>
   <dgm:styleLbl name="parChTrans2D4">
@@ -540,8 +594,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -556,8 +611,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="conFgAcc1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -572,8 +628,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="alignAcc1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -588,8 +645,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="trAlignAcc1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="40000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -604,8 +662,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="bgAcc1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -662,7 +721,7 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAccFollowNode1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
+      <a:schemeClr val="lt1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
@@ -670,7 +729,6 @@
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
-        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -682,7 +740,7 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="alignAccFollowNode1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
+      <a:schemeClr val="lt1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
@@ -690,7 +748,6 @@
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
-        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -702,7 +759,7 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="bgAccFollowNode1">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
+      <a:schemeClr val="lt1">
         <a:alpha val="90000"/>
         <a:tint val="40000"/>
       </a:schemeClr>
@@ -710,7 +767,6 @@
     <dgm:linClrLst meth="repeat">
       <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
-        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:linClrLst>
     <dgm:effectClrLst/>
@@ -722,8 +778,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc0">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -738,8 +795,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc2">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -754,8 +812,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc3">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -770,8 +829,9 @@
   </dgm:styleLbl>
   <dgm:styleLbl name="fgAcc4">
     <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="accent1">
         <a:alpha val="90000"/>
+        <a:tint val="40000"/>
       </a:schemeClr>
     </dgm:fillClrLst>
     <dgm:linClrLst meth="repeat">
@@ -870,758 +930,11 @@
 </dgm:colorsDef>
 </file>
 
-<file path=xl/diagrams/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
-  <dgm:title val=""/>
-  <dgm:desc val=""/>
-  <dgm:catLst>
-    <dgm:cat type="accent1" pri="11200"/>
-  </dgm:catLst>
-  <dgm:styleLbl name="node0">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="lnNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="vennNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgImgPlace1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignImgPlace1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgImgPlace1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgSibTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgSibTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans1D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="callout">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst0">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst/>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:shade val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:shade val="60000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="conFgAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="trAlignAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="40000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="solidFgAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="solidAlignAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="solidBgAcc1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAccFollowNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="90000"/>
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="90000"/>
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignAccFollowNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="90000"/>
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="90000"/>
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgAccFollowNode1">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="90000"/>
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:alpha val="90000"/>
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc0">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc2">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc3">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc4">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="90000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgShp">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="40000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="dkBgShp">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:shade val="80000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="trBgShp">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="50000"/>
-        <a:alpha val="40000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="accent1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgShp">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="accent1">
-        <a:tint val="60000"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="lt1"/>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="dk1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="revTx">
-    <dgm:fillClrLst meth="repeat">
-      <a:schemeClr val="lt1">
-        <a:alpha val="0"/>
-      </a:schemeClr>
-    </dgm:fillClrLst>
-    <dgm:linClrLst meth="repeat">
-      <a:schemeClr val="dk1">
-        <a:alpha val="0"/>
-      </a:schemeClr>
-    </dgm:linClrLst>
-    <dgm:effectClrLst/>
-    <dgm:txLinClrLst/>
-    <dgm:txFillClrLst meth="repeat">
-      <a:schemeClr val="tx1"/>
-    </dgm:txFillClrLst>
-    <dgm:txEffectClrLst/>
-  </dgm:styleLbl>
-</dgm:colorsDef>
-</file>
-
 <file path=xl/diagrams/data1.xml><?xml version="1.0" encoding="utf-8"?>
 <dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <dgm:ptLst>
     <dgm:pt modelId="{6F02A1AC-C5A7-4578-89C1-A6BEC50BF19D}" type="doc">
-      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1" loCatId="hierarchy" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1" loCatId="hierarchy" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple2" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_1" csCatId="accent1" phldr="1"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2492,283 +1805,6 @@
 </dgm:dataModel>
 </file>
 
-<file path=xl/diagrams/data2.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <dgm:ptLst>
-    <dgm:pt modelId="{71312D8E-BAB7-42E4-9119-391F7102B213}" type="doc">
-      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/default" loCatId="list" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="0"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{D1C3D74A-B33F-45B0-AB33-EA354E960E48}">
-      <dgm:prSet phldrT="[文本]" phldr="1"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{5C5BB0F3-6B49-48E7-934F-47FA8CCDA963}" type="parTrans" cxnId="{F1800306-B766-4B3F-942B-4FC7EE23CB81}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{1FC04E78-5C68-414B-ABFA-57906BCD17BF}" type="sibTrans" cxnId="{F1800306-B766-4B3F-942B-4FC7EE23CB81}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{9928AA66-F5D9-413F-8EBF-4F764F918691}">
-      <dgm:prSet phldrT="[文本]" phldr="1"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{F32ED51A-9662-469D-98F7-67C5899F9BD9}" type="parTrans" cxnId="{E8E0A4C5-9188-46D0-B832-3B915A055471}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{2E7AEE7B-AAC5-471B-950C-AB68EB5A21EB}" type="sibTrans" cxnId="{E8E0A4C5-9188-46D0-B832-3B915A055471}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{3AC75ADC-19A7-4ED3-851F-0664DD139C76}">
-      <dgm:prSet phldrT="[文本]" phldr="1"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{7CCB9175-C70E-4F6A-8538-7C9CE8082359}" type="parTrans" cxnId="{09E4B23B-5A00-4554-AB93-B748CC1B9F8C}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{8FAC2696-FF55-4C86-B6EE-435350529519}" type="sibTrans" cxnId="{09E4B23B-5A00-4554-AB93-B748CC1B9F8C}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{C990E1E1-2088-4C2E-B4CD-1884E27C5E2D}">
-      <dgm:prSet phldrT="[文本]" phldr="1"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{BE721ECC-ABA5-494E-8D48-FD1E29D8AFEE}" type="parTrans" cxnId="{BE733ECE-1764-4747-BD4B-DD8D442851FA}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{AD864F94-939C-4CA3-8C37-4BF47C06839A}" type="sibTrans" cxnId="{BE733ECE-1764-4747-BD4B-DD8D442851FA}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{7B38C3B3-A766-4A61-B348-DD4CA82F076B}">
-      <dgm:prSet phldrT="[文本]" phldr="1"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{7A0EF6E1-44B4-4635-9B50-2736BB1B5618}" type="parTrans" cxnId="{CB89C5D3-B8C6-4DF2-A46A-A21351A9B9D5}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{2AC66FD1-4781-4234-9AE4-8F86EB823560}" type="sibTrans" cxnId="{CB89C5D3-B8C6-4DF2-A46A-A21351A9B9D5}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" type="pres">
-      <dgm:prSet presAssocID="{71312D8E-BAB7-42E4-9119-391F7102B213}" presName="diagram" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:dir/>
-          <dgm:resizeHandles val="exact"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9488F2AF-59B1-4D11-8C22-494D08204D5D}" type="pres">
-      <dgm:prSet presAssocID="{D1C3D74A-B33F-45B0-AB33-EA354E960E48}" presName="node" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:bulletEnabled val="1"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{87708114-C1B7-4D1E-88A9-C7D85B7CE12E}" type="pres">
-      <dgm:prSet presAssocID="{1FC04E78-5C68-414B-ABFA-57906BCD17BF}" presName="sibTrans" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{4098D9E8-6B8F-47F0-96E6-66F38BE99DDF}" type="pres">
-      <dgm:prSet presAssocID="{9928AA66-F5D9-413F-8EBF-4F764F918691}" presName="node" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:bulletEnabled val="1"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2819DFF7-810B-4DDE-B64F-7D10A0409824}" type="pres">
-      <dgm:prSet presAssocID="{2E7AEE7B-AAC5-471B-950C-AB68EB5A21EB}" presName="sibTrans" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F15B32AC-2F7D-4E0D-AF3E-7CC0A69E60EE}" type="pres">
-      <dgm:prSet presAssocID="{3AC75ADC-19A7-4ED3-851F-0664DD139C76}" presName="node" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:bulletEnabled val="1"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{A00C783A-53AE-490C-BA1E-E4B3C7A227AF}" type="pres">
-      <dgm:prSet presAssocID="{8FAC2696-FF55-4C86-B6EE-435350529519}" presName="sibTrans" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{21C0A888-AE9E-4B94-B9CD-077B60BB8092}" type="pres">
-      <dgm:prSet presAssocID="{C990E1E1-2088-4C2E-B4CD-1884E27C5E2D}" presName="node" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:bulletEnabled val="1"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{19B3F08C-F181-4A23-8456-0B76F281679D}" type="pres">
-      <dgm:prSet presAssocID="{AD864F94-939C-4CA3-8C37-4BF47C06839A}" presName="sibTrans" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B44A85B9-6567-4EFD-90D3-BA82E28968A0}" type="pres">
-      <dgm:prSet presAssocID="{7B38C3B3-A766-4A61-B348-DD4CA82F076B}" presName="node" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:bulletEnabled val="1"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-  </dgm:ptLst>
-  <dgm:cxnLst>
-    <dgm:cxn modelId="{F1800306-B766-4B3F-942B-4FC7EE23CB81}" srcId="{71312D8E-BAB7-42E4-9119-391F7102B213}" destId="{D1C3D74A-B33F-45B0-AB33-EA354E960E48}" srcOrd="0" destOrd="0" parTransId="{5C5BB0F3-6B49-48E7-934F-47FA8CCDA963}" sibTransId="{1FC04E78-5C68-414B-ABFA-57906BCD17BF}"/>
-    <dgm:cxn modelId="{B348131A-195A-49AE-AF7F-1000C040E97F}" type="presOf" srcId="{3AC75ADC-19A7-4ED3-851F-0664DD139C76}" destId="{F15B32AC-2F7D-4E0D-AF3E-7CC0A69E60EE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{09E4B23B-5A00-4554-AB93-B748CC1B9F8C}" srcId="{71312D8E-BAB7-42E4-9119-391F7102B213}" destId="{3AC75ADC-19A7-4ED3-851F-0664DD139C76}" srcOrd="2" destOrd="0" parTransId="{7CCB9175-C70E-4F6A-8538-7C9CE8082359}" sibTransId="{8FAC2696-FF55-4C86-B6EE-435350529519}"/>
-    <dgm:cxn modelId="{1CFE3747-67B2-415E-AB1D-C57907A65B09}" type="presOf" srcId="{C990E1E1-2088-4C2E-B4CD-1884E27C5E2D}" destId="{21C0A888-AE9E-4B94-B9CD-077B60BB8092}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{AA2E3C6F-65D5-430E-BF67-89F37F7517EB}" type="presOf" srcId="{D1C3D74A-B33F-45B0-AB33-EA354E960E48}" destId="{9488F2AF-59B1-4D11-8C22-494D08204D5D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{91F15D7F-244A-48A0-B21B-AEA509A02B0F}" type="presOf" srcId="{9928AA66-F5D9-413F-8EBF-4F764F918691}" destId="{4098D9E8-6B8F-47F0-96E6-66F38BE99DDF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{0A74DCA7-1BE6-41FF-A1EF-B7B9668E5C58}" type="presOf" srcId="{7B38C3B3-A766-4A61-B348-DD4CA82F076B}" destId="{B44A85B9-6567-4EFD-90D3-BA82E28968A0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{E8E0A4C5-9188-46D0-B832-3B915A055471}" srcId="{71312D8E-BAB7-42E4-9119-391F7102B213}" destId="{9928AA66-F5D9-413F-8EBF-4F764F918691}" srcOrd="1" destOrd="0" parTransId="{F32ED51A-9662-469D-98F7-67C5899F9BD9}" sibTransId="{2E7AEE7B-AAC5-471B-950C-AB68EB5A21EB}"/>
-    <dgm:cxn modelId="{BE733ECE-1764-4747-BD4B-DD8D442851FA}" srcId="{71312D8E-BAB7-42E4-9119-391F7102B213}" destId="{C990E1E1-2088-4C2E-B4CD-1884E27C5E2D}" srcOrd="3" destOrd="0" parTransId="{BE721ECC-ABA5-494E-8D48-FD1E29D8AFEE}" sibTransId="{AD864F94-939C-4CA3-8C37-4BF47C06839A}"/>
-    <dgm:cxn modelId="{8F84B9CE-83FB-4DD8-BDD0-FBEFB55D71A8}" type="presOf" srcId="{71312D8E-BAB7-42E4-9119-391F7102B213}" destId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{CB89C5D3-B8C6-4DF2-A46A-A21351A9B9D5}" srcId="{71312D8E-BAB7-42E4-9119-391F7102B213}" destId="{7B38C3B3-A766-4A61-B348-DD4CA82F076B}" srcOrd="4" destOrd="0" parTransId="{7A0EF6E1-44B4-4635-9B50-2736BB1B5618}" sibTransId="{2AC66FD1-4781-4234-9AE4-8F86EB823560}"/>
-    <dgm:cxn modelId="{211499DE-4366-4789-9BD1-2E6E962EC634}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{9488F2AF-59B1-4D11-8C22-494D08204D5D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{EF4FDEF6-743B-40D7-8C2E-56E3CC19F42A}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{87708114-C1B7-4D1E-88A9-C7D85B7CE12E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{4043A454-B5DB-4457-8F1A-CE4A92F36D82}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{4098D9E8-6B8F-47F0-96E6-66F38BE99DDF}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{6339A1AC-1E31-4B9F-B98C-5334A0EFE476}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{2819DFF7-810B-4DDE-B64F-7D10A0409824}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{3F411D1B-2649-4BEA-9734-BDA519E8D403}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{F15B32AC-2F7D-4E0D-AF3E-7CC0A69E60EE}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{B8192E83-F3AD-4CA7-AB09-DAFD3E5A775F}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{A00C783A-53AE-490C-BA1E-E4B3C7A227AF}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{22B9E86E-F242-41AD-8C18-9A5442D8B1C6}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{21C0A888-AE9E-4B94-B9CD-077B60BB8092}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{AAC3F5DD-2706-4239-BDE4-042D67ACC678}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{19B3F08C-F181-4A23-8456-0B76F281679D}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{030E2DEA-F393-4F8F-88AF-D3D8A7C3EC7D}" type="presParOf" srcId="{FCD5B019-6354-4FB8-850E-32EBC43EF24D}" destId="{B44A85B9-6567-4EFD-90D3-BA82E28968A0}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-  </dgm:cxnLst>
-  <dgm:bg/>
-  <dgm:whole/>
-  <dgm:extLst>
-    <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
-      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId10" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-    </a:ext>
-  </dgm:extLst>
-</dgm:dataModel>
-</file>
-
 <file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <dsp:spTree>
@@ -2784,8 +1820,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4036336" y="1025601"/>
-          <a:ext cx="127065" cy="1592554"/>
+          <a:off x="4006306" y="1036899"/>
+          <a:ext cx="128541" cy="1611049"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2799,10 +1835,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="1592554"/>
+                <a:pt x="0" y="1611049"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="127065" y="1592554"/>
+                <a:pt x="128541" y="1611049"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2843,8 +1879,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4036336" y="1025601"/>
-          <a:ext cx="127065" cy="991111"/>
+          <a:off x="4006306" y="1036899"/>
+          <a:ext cx="128541" cy="1002621"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2858,10 +1894,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="991111"/>
+                <a:pt x="0" y="1002621"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="127065" y="991111"/>
+                <a:pt x="128541" y="1002621"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2902,8 +1938,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4036336" y="1025601"/>
-          <a:ext cx="127065" cy="389667"/>
+          <a:off x="4006306" y="1036899"/>
+          <a:ext cx="128541" cy="394192"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2917,10 +1953,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="389667"/>
+                <a:pt x="0" y="394192"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="127065" y="389667"/>
+                <a:pt x="128541" y="394192"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2961,8 +1997,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3350182" y="424158"/>
-          <a:ext cx="1024995" cy="177891"/>
+          <a:off x="3312184" y="428470"/>
+          <a:ext cx="1036898" cy="179957"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2976,13 +2012,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="88945"/>
+                <a:pt x="0" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1024995" y="88945"/>
+                <a:pt x="1036898" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1024995" y="177891"/>
+                <a:pt x="1036898" y="179957"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3023,8 +2059,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3011341" y="1627045"/>
-          <a:ext cx="127065" cy="389667"/>
+          <a:off x="2969407" y="1645327"/>
+          <a:ext cx="128541" cy="394192"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3038,10 +2074,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="389667"/>
+                <a:pt x="0" y="394192"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="127065" y="389667"/>
+                <a:pt x="128541" y="394192"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3082,8 +2118,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2325187" y="1025601"/>
-          <a:ext cx="1024995" cy="177891"/>
+          <a:off x="2275285" y="1036899"/>
+          <a:ext cx="1036898" cy="179957"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3097,13 +2133,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="88945"/>
+                <a:pt x="0" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1024995" y="88945"/>
+                <a:pt x="1036898" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1024995" y="177891"/>
+                <a:pt x="1036898" y="179957"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3144,8 +2180,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2279467" y="1025601"/>
-          <a:ext cx="91440" cy="177891"/>
+          <a:off x="2229565" y="1036899"/>
+          <a:ext cx="91440" cy="179957"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3159,7 +2195,7 @@
                 <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="45720" y="177891"/>
+                <a:pt x="45720" y="179957"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3200,8 +2236,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1300191" y="1025601"/>
-          <a:ext cx="1024995" cy="177891"/>
+          <a:off x="1238386" y="1036899"/>
+          <a:ext cx="1036898" cy="179957"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3212,16 +2248,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1024995" y="0"/>
+                <a:pt x="1036898" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1024995" y="88945"/>
+                <a:pt x="1036898" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="88945"/>
+                <a:pt x="0" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="177891"/>
+                <a:pt x="0" y="179957"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3262,8 +2298,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2325187" y="424158"/>
-          <a:ext cx="1024995" cy="177891"/>
+          <a:off x="2275285" y="428470"/>
+          <a:ext cx="1036898" cy="179957"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3274,16 +2310,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1024995" y="0"/>
+                <a:pt x="1036898" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1024995" y="88945"/>
+                <a:pt x="1036898" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="88945"/>
+                <a:pt x="0" y="89978"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="177891"/>
+                <a:pt x="0" y="179957"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3324,23 +2360,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2926630" y="606"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="2883713" y="0"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3353,13 +2390,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3392,8 +2429,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2926630" y="606"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="2883713" y="0"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{469D4EAF-3CDB-43B4-BCB0-38C0E2BD6C87}">
@@ -3403,23 +2440,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1901635" y="602049"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="1846814" y="608428"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3432,13 +2470,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3471,8 +2509,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1901635" y="602049"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="1846814" y="608428"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B703FCFA-C24A-4979-892C-83458DD7006F}">
@@ -3482,23 +2520,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="876640" y="1203493"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="809915" y="1216856"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3511,13 +2550,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3550,8 +2589,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="876640" y="1203493"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="809915" y="1216856"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{592523D9-2D98-4CAA-A045-351A1F014421}">
@@ -3561,23 +2600,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1901635" y="1203493"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="1846814" y="1216856"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3590,13 +2630,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3629,8 +2669,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1901635" y="1203493"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="1846814" y="1216856"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C19FDC6B-23E9-4454-9CF5-5D3E221F356B}">
@@ -3640,23 +2680,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2926630" y="1203493"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="2883713" y="1216856"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3669,13 +2710,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3708,8 +2749,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2926630" y="1203493"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="2883713" y="1216856"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{5CE7488E-A24E-40E2-86A3-2020786F5935}">
@@ -3719,23 +2760,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3138406" y="1804937"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="3097948" y="1825284"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3748,13 +2790,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3787,8 +2829,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3138406" y="1804937"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="3097948" y="1825284"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{BC69C81A-0EBB-4A14-B4B8-A42DAF2C71CF}">
@@ -3798,23 +2840,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3951626" y="602049"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="3920612" y="608428"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3827,13 +2870,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3866,8 +2909,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3951626" y="602049"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="3920612" y="608428"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{34A882B4-7973-48AC-98B3-077EBD67E328}">
@@ -3877,23 +2920,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4163402" y="1203493"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="4134847" y="1216856"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3906,13 +2950,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -3945,8 +2989,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4163402" y="1203493"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="4134847" y="1216856"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E2FA1C5F-FA5B-4B25-9E96-67D9F16B4427}">
@@ -3956,23 +3000,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4163402" y="1804937"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="4134847" y="1825284"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -3985,13 +3030,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -4024,8 +3069,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4163402" y="1804937"/>
-        <a:ext cx="847103" cy="423551"/>
+        <a:off x="4134847" y="1825284"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{80EBFA80-9630-42B8-99AA-91F7FDCD9057}">
@@ -4035,23 +3080,24 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4163402" y="2406380"/>
-          <a:ext cx="847103" cy="423551"/>
+          <a:off x="4134847" y="2433713"/>
+          <a:ext cx="856941" cy="428470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="lt1">
             <a:hueOff val="0"/>
             <a:satOff val="0"/>
             <a:lumOff val="0"/>
             <a:alphaOff val="0"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4064,13 +3110,13 @@
         <a:effectLst/>
       </dsp:spPr>
       <dsp:style>
-        <a:lnRef idx="2">
+        <a:lnRef idx="3">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="0">
+        <a:effectRef idx="1">
           <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
@@ -4103,395 +3149,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4163402" y="2406380"/>
-        <a:ext cx="847103" cy="423551"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-  </dsp:spTree>
-</dsp:drawing>
-</file>
-
-<file path=xl/diagrams/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <dsp:spTree>
-    <dsp:nvGrpSpPr>
-      <dsp:cNvPr id="0" name=""/>
-      <dsp:cNvGrpSpPr/>
-    </dsp:nvGrpSpPr>
-    <dsp:grpSpPr/>
-    <dsp:sp modelId="{9488F2AF-59B1-4D11-8C22-494D08204D5D}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="0" y="442912"/>
-          <a:ext cx="1428749" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="137160" tIns="137160" rIns="137160" bIns="137160" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="3600" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="0" y="442912"/>
-        <a:ext cx="1428749" cy="857250"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{4098D9E8-6B8F-47F0-96E6-66F38BE99DDF}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1571625" y="442912"/>
-          <a:ext cx="1428749" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="137160" tIns="137160" rIns="137160" bIns="137160" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="3600" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="1571625" y="442912"/>
-        <a:ext cx="1428749" cy="857250"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F15B32AC-2F7D-4E0D-AF3E-7CC0A69E60EE}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3143250" y="442912"/>
-          <a:ext cx="1428749" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="137160" tIns="137160" rIns="137160" bIns="137160" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="3600" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3143250" y="442912"/>
-        <a:ext cx="1428749" cy="857250"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{21C0A888-AE9E-4B94-B9CD-077B60BB8092}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="785812" y="1443037"/>
-          <a:ext cx="1428749" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="137160" tIns="137160" rIns="137160" bIns="137160" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="3600" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="785812" y="1443037"/>
-        <a:ext cx="1428749" cy="857250"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{B44A85B9-6567-4EFD-90D3-BA82E28968A0}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2357437" y="1443037"/>
-          <a:ext cx="1428749" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="137160" tIns="137160" rIns="137160" bIns="137160" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="3600" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2357437" y="1443037"/>
-        <a:ext cx="1428749" cy="857250"/>
+        <a:off x="4134847" y="2433713"/>
+        <a:ext cx="856941" cy="428470"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -5644,159 +4303,12 @@
 </dgm:layoutDef>
 </file>
 
-<file path=xl/diagrams/layout2.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:layoutDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/layout/default">
+<file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple2">
   <dgm:title val=""/>
   <dgm:desc val=""/>
   <dgm:catLst>
-    <dgm:cat type="list" pri="400"/>
-  </dgm:catLst>
-  <dgm:sampData>
-    <dgm:dataModel>
-      <dgm:ptLst>
-        <dgm:pt modelId="0" type="doc"/>
-        <dgm:pt modelId="1">
-          <dgm:prSet phldr="1"/>
-        </dgm:pt>
-        <dgm:pt modelId="2">
-          <dgm:prSet phldr="1"/>
-        </dgm:pt>
-        <dgm:pt modelId="3">
-          <dgm:prSet phldr="1"/>
-        </dgm:pt>
-        <dgm:pt modelId="4">
-          <dgm:prSet phldr="1"/>
-        </dgm:pt>
-        <dgm:pt modelId="5">
-          <dgm:prSet phldr="1"/>
-        </dgm:pt>
-      </dgm:ptLst>
-      <dgm:cxnLst>
-        <dgm:cxn modelId="6" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
-        <dgm:cxn modelId="7" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
-        <dgm:cxn modelId="8" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
-        <dgm:cxn modelId="9" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
-        <dgm:cxn modelId="10" srcId="0" destId="5" srcOrd="4" destOrd="0"/>
-      </dgm:cxnLst>
-      <dgm:bg/>
-      <dgm:whole/>
-    </dgm:dataModel>
-  </dgm:sampData>
-  <dgm:styleData>
-    <dgm:dataModel>
-      <dgm:ptLst>
-        <dgm:pt modelId="0" type="doc"/>
-        <dgm:pt modelId="1"/>
-        <dgm:pt modelId="2"/>
-      </dgm:ptLst>
-      <dgm:cxnLst>
-        <dgm:cxn modelId="3" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
-        <dgm:cxn modelId="4" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
-      </dgm:cxnLst>
-      <dgm:bg/>
-      <dgm:whole/>
-    </dgm:dataModel>
-  </dgm:styleData>
-  <dgm:clrData>
-    <dgm:dataModel>
-      <dgm:ptLst>
-        <dgm:pt modelId="0" type="doc"/>
-        <dgm:pt modelId="1"/>
-        <dgm:pt modelId="2"/>
-        <dgm:pt modelId="3"/>
-        <dgm:pt modelId="4"/>
-        <dgm:pt modelId="5"/>
-        <dgm:pt modelId="6"/>
-      </dgm:ptLst>
-      <dgm:cxnLst>
-        <dgm:cxn modelId="7" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
-        <dgm:cxn modelId="8" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
-        <dgm:cxn modelId="9" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
-        <dgm:cxn modelId="10" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
-        <dgm:cxn modelId="11" srcId="0" destId="5" srcOrd="4" destOrd="0"/>
-        <dgm:cxn modelId="12" srcId="0" destId="6" srcOrd="5" destOrd="0"/>
-      </dgm:cxnLst>
-      <dgm:bg/>
-      <dgm:whole/>
-    </dgm:dataModel>
-  </dgm:clrData>
-  <dgm:layoutNode name="diagram">
-    <dgm:varLst>
-      <dgm:dir/>
-      <dgm:resizeHandles val="exact"/>
-    </dgm:varLst>
-    <dgm:choose name="Name0">
-      <dgm:if name="Name1" func="var" arg="dir" op="equ" val="norm">
-        <dgm:alg type="snake">
-          <dgm:param type="grDir" val="tL"/>
-          <dgm:param type="flowDir" val="row"/>
-          <dgm:param type="contDir" val="sameDir"/>
-          <dgm:param type="off" val="ctr"/>
-        </dgm:alg>
-      </dgm:if>
-      <dgm:else name="Name2">
-        <dgm:alg type="snake">
-          <dgm:param type="grDir" val="tR"/>
-          <dgm:param type="flowDir" val="row"/>
-          <dgm:param type="contDir" val="sameDir"/>
-          <dgm:param type="off" val="ctr"/>
-        </dgm:alg>
-      </dgm:else>
-    </dgm:choose>
-    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
-      <dgm:adjLst/>
-    </dgm:shape>
-    <dgm:presOf/>
-    <dgm:constrLst>
-      <dgm:constr type="w" for="ch" forName="node" refType="w"/>
-      <dgm:constr type="h" for="ch" forName="node" refType="w" refFor="ch" refForName="node" fact="0.6"/>
-      <dgm:constr type="w" for="ch" forName="sibTrans" refType="w" refFor="ch" refForName="node" fact="0.1"/>
-      <dgm:constr type="sp" refType="w" refFor="ch" refForName="sibTrans"/>
-      <dgm:constr type="primFontSz" for="ch" forName="node" op="equ" val="65"/>
-    </dgm:constrLst>
-    <dgm:ruleLst/>
-    <dgm:forEach name="Name3" axis="ch" ptType="node">
-      <dgm:layoutNode name="node">
-        <dgm:varLst>
-          <dgm:bulletEnabled val="1"/>
-        </dgm:varLst>
-        <dgm:alg type="tx"/>
-        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="rect" r:blip="">
-          <dgm:adjLst/>
-        </dgm:shape>
-        <dgm:presOf axis="desOrSelf" ptType="node"/>
-        <dgm:constrLst>
-          <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
-          <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
-          <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
-          <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
-        </dgm:constrLst>
-        <dgm:ruleLst>
-          <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
-        </dgm:ruleLst>
-      </dgm:layoutNode>
-      <dgm:forEach name="Name4" axis="followSib" ptType="sibTrans" cnt="1">
-        <dgm:layoutNode name="sibTrans">
-          <dgm:alg type="sp"/>
-          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
-            <dgm:adjLst/>
-          </dgm:shape>
-          <dgm:presOf/>
-          <dgm:constrLst/>
-          <dgm:ruleLst/>
-        </dgm:layoutNode>
-      </dgm:forEach>
-    </dgm:forEach>
-  </dgm:layoutNode>
-</dgm:layoutDef>
-</file>
-
-<file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
-  <dgm:title val=""/>
-  <dgm:desc val=""/>
-  <dgm:catLst>
-    <dgm:cat type="simple" pri="10100"/>
+    <dgm:cat type="simple" pri="10200"/>
   </dgm:catLst>
   <dgm:scene3d>
     <a:camera prst="orthographicFront"/>
@@ -5810,13 +4322,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5832,13 +4344,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5854,7 +4366,7 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
@@ -5882,7 +4394,7 @@
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5898,13 +4410,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5920,13 +4432,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5942,13 +4454,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5964,13 +4476,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -5986,13 +4498,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor"/>
@@ -6006,13 +4518,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor"/>
@@ -6026,13 +4538,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor"/>
@@ -6052,7 +4564,7 @@
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6074,7 +4586,7 @@
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6096,7 +4608,7 @@
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6138,7 +4650,7 @@
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor"/>
@@ -6152,13 +4664,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6174,13 +4686,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6196,13 +4708,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6218,13 +4730,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6240,13 +4752,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6262,13 +4774,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6284,13 +4796,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6306,13 +4818,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6328,13 +4840,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor">
@@ -6790,13 +5302,13 @@
     <dgm:sp3d/>
     <dgm:txPr/>
     <dgm:style>
-      <a:lnRef idx="2">
+      <a:lnRef idx="3">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:lnRef>
       <a:fillRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:fillRef>
-      <a:effectRef idx="0">
+      <a:effectRef idx="1">
         <a:scrgbClr r="0" g="0" b="0"/>
       </a:effectRef>
       <a:fontRef idx="minor"/>
@@ -6825,1054 +5337,20 @@
 </dgm:styleDef>
 </file>
 
-<file path=xl/diagrams/quickStyle2.xml><?xml version="1.0" encoding="utf-8"?>
-<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
-  <dgm:title val=""/>
-  <dgm:desc val=""/>
-  <dgm:catLst>
-    <dgm:cat type="simple" pri="10100"/>
-  </dgm:catLst>
-  <dgm:scene3d>
-    <a:camera prst="orthographicFront"/>
-    <a:lightRig rig="threePt" dir="t"/>
-  </dgm:scene3d>
-  <dgm:styleLbl name="node0">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="lnNode1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="vennNode1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="tx1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignNode1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node2">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node3">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="node4">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgImgPlace1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignImgPlace1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgImgPlace1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans2D1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgSibTrans2D1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgSibTrans2D1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="sibTrans1D1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="callout">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst0">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst2">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst3">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="asst4">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D2">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D3">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans2D4">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor">
-        <a:schemeClr val="lt1"/>
-      </a:fontRef>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D2">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D3">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="parChTrans1D4">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="conFgAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="trAlignAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="solidFgAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="solidAlignAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="solidBgAcc1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAccFollowNode1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="alignAccFollowNode1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgAccFollowNode1">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc0">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc2">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc3">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgAcc4">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="bgShp">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="dkBgShp">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="trBgShp">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="fgShp">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="2">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="1">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-  <dgm:styleLbl name="revTx">
-    <dgm:scene3d>
-      <a:camera prst="orthographicFront"/>
-      <a:lightRig rig="threePt" dir="t"/>
-    </dgm:scene3d>
-    <dgm:sp3d/>
-    <dgm:txPr/>
-    <dgm:style>
-      <a:lnRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:lnRef>
-      <a:fillRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:fillRef>
-      <a:effectRef idx="0">
-        <a:scrgbClr r="0" g="0" b="0"/>
-      </a:effectRef>
-      <a:fontRef idx="minor"/>
-    </dgm:style>
-  </dgm:styleLbl>
-</dgm:styleDef>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>17467</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>84176</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>193031</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>66453</xdr:rowOff>
+      <xdr:colOff>392393</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>77528</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7897,43 +5375,19 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>88921</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>483844</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>165943</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="图示 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7431EBCC-0CEA-98B9-DC96-925E06B5EB39}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
-          <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId6" r:lo="rId7" r:qs="rId8" r:cs="rId9"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2E94850-7600-4CE4-B7BF-DA13FA39E1CA}" name="表1" displayName="表1" ref="K2:M5" totalsRowShown="0">
+  <autoFilter ref="K2:M5" xr:uid="{A2E94850-7600-4CE4-B7BF-DA13FA39E1CA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{050706C5-6B03-4257-BFFB-D44995C3349C}" name="WebStatemachine"/>
+    <tableColumn id="2" xr3:uid="{0CB8C68D-C40C-42AF-AC25-D03E823A9A29}" name="Unsign in state"/>
+    <tableColumn id="3" xr3:uid="{DA51DA47-DA47-4186-91CB-AA8E48FE6B0F}" name="Sign in state"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8236,45 +5690,46 @@
   <dimension ref="K2:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="24.2109375" customWidth="1"/>
+    <col min="11" max="11" width="24.25" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="11:13" ht="20.149999999999999" x14ac:dyDescent="0.5">
+    <row r="2" spans="11:13" ht="20.25" x14ac:dyDescent="0.3">
       <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="11:13" x14ac:dyDescent="0.35">
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
+    <row r="5" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="11:13" x14ac:dyDescent="0.35">
-      <c r="L4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="11:13" x14ac:dyDescent="0.35">
-      <c r="M5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -8282,5 +5737,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>